<commit_message>
worked on microcontroller schematics
</commit_message>
<xml_diff>
--- a/RD40_electronics/RD40_display_SMD_V1/JLCPCB_BOM.xlsx
+++ b/RD40_electronics/RD40_display_SMD_V1/JLCPCB_BOM.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lbmon\Elektronik\rotating_display\RD40_electronics\RD40_display_SMD_V1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2929C72B-30C0-4FD7-80B7-9CF2215BA633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14628D4F-8E98-4A64-A219-101B1FB517AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12336" xr2:uid="{8BD6F50D-B285-458D-A48B-800F3747C71B}"/>
+    <workbookView xWindow="24" yWindow="624" windowWidth="23016" windowHeight="12336" xr2:uid="{8BD6F50D-B285-458D-A48B-800F3747C71B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="75">
   <si>
     <t>JLCPCB Parts List</t>
   </si>
@@ -69,6 +70,198 @@
   </si>
   <si>
     <t>6000K~7000K 1300mcd Yellow Diffused -40℃~+85℃ Positive post White light 140° 102mW 1206  Light Emitting Diodes (LED) ROHS</t>
+  </si>
+  <si>
+    <t>16 MHz crystal</t>
+  </si>
+  <si>
+    <t>part</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>C1, C2</t>
+  </si>
+  <si>
+    <t>C1547</t>
+  </si>
+  <si>
+    <t>12pF</t>
+  </si>
+  <si>
+    <t>FH (Guangdong Fenghua Advanced Tech)</t>
+  </si>
+  <si>
+    <t>0402CG120J500NT</t>
+  </si>
+  <si>
+    <t>C13738</t>
+  </si>
+  <si>
+    <t>standard</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Yangxing Tech</t>
+  </si>
+  <si>
+    <t>X322516MLB4SI</t>
+  </si>
+  <si>
+    <t>ATMEGA328P-AU</t>
+  </si>
+  <si>
+    <t>C14877</t>
+  </si>
+  <si>
+    <t>Microchip Tech</t>
+  </si>
+  <si>
+    <t>0402</t>
+  </si>
+  <si>
+    <t>10kΩ</t>
+  </si>
+  <si>
+    <t>UNI-ROYAL(Uniroyal Elec)</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>100nF</t>
+  </si>
+  <si>
+    <t>C14663</t>
+  </si>
+  <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t>CC0603KRX7R9BB104</t>
+  </si>
+  <si>
+    <t>C307331</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics</t>
+  </si>
+  <si>
+    <t>CL05B104KB54PNC</t>
+  </si>
+  <si>
+    <t>C25744</t>
+  </si>
+  <si>
+    <t>0402WGF1002TCE</t>
+  </si>
+  <si>
+    <t>R1, R2, R3</t>
+  </si>
+  <si>
+    <t>WCH(Jiangsu Qin Heng)</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>SHOU HAN</t>
+  </si>
+  <si>
+    <t>CH340C</t>
+  </si>
+  <si>
+    <t>C7464026</t>
+  </si>
+  <si>
+    <t>C8598</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>Schottky</t>
+  </si>
+  <si>
+    <t>Jiangsu Changjing Electronics Technology Co., Ltd.</t>
+  </si>
+  <si>
+    <t>B5819W SL</t>
+  </si>
+  <si>
+    <t>40V 600mV@1A 1A SOD-123 Schottky Barrier Diodes (SBD) ROHS</t>
+  </si>
+  <si>
+    <t>USB micro</t>
+  </si>
+  <si>
+    <t>C2681557</t>
+  </si>
+  <si>
+    <t>MICRO QTZB5.5</t>
+  </si>
+  <si>
+    <t>USB 2.0 1 Surface Mount 5P Female -30℃~+85℃ Micro-B SMD USB Connectors ROHS</t>
+  </si>
+  <si>
+    <t>10µF</t>
+  </si>
+  <si>
+    <t>C15850</t>
+  </si>
+  <si>
+    <t>0805</t>
+  </si>
+  <si>
+    <t>CL21A106KAYNNNE</t>
+  </si>
+  <si>
+    <t>C350572</t>
+  </si>
+  <si>
+    <t>TPIC6C595</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>TPIC6C595DR</t>
+  </si>
+  <si>
+    <t>8 4.5V~5.5V 1 串行至并行或串行 SOIC-16 Shifting Register ROHS</t>
+  </si>
+  <si>
+    <t>C10, C11, C13, C15</t>
+  </si>
+  <si>
+    <t>C4, C5, C6, C7, C8, C9, C12, C14</t>
+  </si>
+  <si>
+    <t>ESP-12F</t>
+  </si>
+  <si>
+    <t>C82891</t>
+  </si>
+  <si>
+    <t>Ai-Thinker</t>
+  </si>
+  <si>
+    <t>ESP-12F(ESP8266MOD)</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>U3, U5</t>
   </si>
 </sst>
 </file>
@@ -126,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -135,6 +328,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -451,58 +647,329 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E83B5D-4541-480F-8D66-7615F800B320}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="43" customWidth="1"/>
-    <col min="4" max="4" width="29.21875" customWidth="1"/>
-    <col min="5" max="5" width="61.21875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
+    <col min="5" max="5" width="43" customWidth="1"/>
+    <col min="6" max="6" width="29.21875" customWidth="1"/>
+    <col min="7" max="7" width="61.21875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="29.4" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:7" ht="29.4" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="43.8" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="29.4" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SMD circuit diagram further completed
</commit_message>
<xml_diff>
--- a/RD40_electronics/RD40_display_SMD_V1/JLCPCB_BOM.xlsx
+++ b/RD40_electronics/RD40_display_SMD_V1/JLCPCB_BOM.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lbmon\Elektronik\rotating_display\RD40_electronics\RD40_display_SMD_V1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14628D4F-8E98-4A64-A219-101B1FB517AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2011C638-FD5B-42B3-B32D-1147E20F06F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="624" windowWidth="23016" windowHeight="12336" xr2:uid="{8BD6F50D-B285-458D-A48B-800F3747C71B}"/>
+    <workbookView xWindow="24" yWindow="24" windowWidth="22968" windowHeight="12336" xr2:uid="{8BD6F50D-B285-458D-A48B-800F3747C71B}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="110">
   <si>
     <t>JLCPCB Parts List</t>
   </si>
@@ -135,21 +134,9 @@
     <t>0603</t>
   </si>
   <si>
-    <t>C3</t>
-  </si>
-  <si>
     <t>100nF</t>
   </si>
   <si>
-    <t>C14663</t>
-  </si>
-  <si>
-    <t>YAGEO</t>
-  </si>
-  <si>
-    <t>CC0603KRX7R9BB104</t>
-  </si>
-  <si>
     <t>C307331</t>
   </si>
   <si>
@@ -165,18 +152,12 @@
     <t>0402WGF1002TCE</t>
   </si>
   <si>
-    <t>R1, R2, R3</t>
-  </si>
-  <si>
     <t>WCH(Jiangsu Qin Heng)</t>
   </si>
   <si>
     <t>P1</t>
   </si>
   <si>
-    <t>SHOU HAN</t>
-  </si>
-  <si>
     <t>CH340C</t>
   </si>
   <si>
@@ -186,9 +167,6 @@
     <t>C8598</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
     <t>Schottky</t>
   </si>
   <si>
@@ -201,21 +179,6 @@
     <t>40V 600mV@1A 1A SOD-123 Schottky Barrier Diodes (SBD) ROHS</t>
   </si>
   <si>
-    <t>USB micro</t>
-  </si>
-  <si>
-    <t>C2681557</t>
-  </si>
-  <si>
-    <t>MICRO QTZB5.5</t>
-  </si>
-  <si>
-    <t>USB 2.0 1 Surface Mount 5P Female -30℃~+85℃ Micro-B SMD USB Connectors ROHS</t>
-  </si>
-  <si>
-    <t>10µF</t>
-  </si>
-  <si>
     <t>C15850</t>
   </si>
   <si>
@@ -240,12 +203,6 @@
     <t>8 4.5V~5.5V 1 串行至并行或串行 SOIC-16 Shifting Register ROHS</t>
   </si>
   <si>
-    <t>C10, C11, C13, C15</t>
-  </si>
-  <si>
-    <t>C4, C5, C6, C7, C8, C9, C12, C14</t>
-  </si>
-  <si>
     <t>ESP-12F</t>
   </si>
   <si>
@@ -258,10 +215,157 @@
     <t>ESP-12F(ESP8266MOD)</t>
   </si>
   <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>U3, U5</t>
+    <t>22µF, 25V</t>
+  </si>
+  <si>
+    <t>C45783</t>
+  </si>
+  <si>
+    <t>CL21A226MAQNNNE</t>
+  </si>
+  <si>
+    <t>C15008</t>
+  </si>
+  <si>
+    <t>100µF, 6,3V</t>
+  </si>
+  <si>
+    <t>C96123</t>
+  </si>
+  <si>
+    <t>47µF, 10V</t>
+  </si>
+  <si>
+    <t>1117 5.0</t>
+  </si>
+  <si>
+    <t>C6187</t>
+  </si>
+  <si>
+    <t>SOT-223</t>
+  </si>
+  <si>
+    <t>C6186</t>
+  </si>
+  <si>
+    <t>1117 3.3</t>
+  </si>
+  <si>
+    <t>SOT-223-3</t>
+  </si>
+  <si>
+    <t>C709357</t>
+  </si>
+  <si>
+    <t>USB-C</t>
+  </si>
+  <si>
+    <t>Shenzhen Kinghelm Elec</t>
+  </si>
+  <si>
+    <t>KH-TYPE-C-16P</t>
+  </si>
+  <si>
+    <t>C25905</t>
+  </si>
+  <si>
+    <t>5.1 kΩ</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>Q1, Q2</t>
+  </si>
+  <si>
+    <t>C2146</t>
+  </si>
+  <si>
+    <t>J3Y</t>
+  </si>
+  <si>
+    <t>C24, C25</t>
+  </si>
+  <si>
+    <t>C3, C4</t>
+  </si>
+  <si>
+    <t>C5, C6, C7, C8</t>
+  </si>
+  <si>
+    <t>10µF, 10V</t>
+  </si>
+  <si>
+    <t>1206</t>
+  </si>
+  <si>
+    <t>10µF, 25V</t>
+  </si>
+  <si>
+    <t>C19702</t>
+  </si>
+  <si>
+    <t>C12, C17, C21</t>
+  </si>
+  <si>
+    <t>C9, C13</t>
+  </si>
+  <si>
+    <t>C10, C11, C14, C15, C16, C18, C19, C20, C22, C23, C26, C27, C28, C29, C30, C31</t>
+  </si>
+  <si>
+    <t>D1, D2, D3, D4, D5, D6</t>
+  </si>
+  <si>
+    <t>D7, …, D46</t>
+  </si>
+  <si>
+    <t>R1, R2, R5, R7, R8, R13, R14, R15</t>
+  </si>
+  <si>
+    <t>R3, R4, R9, R10</t>
+  </si>
+  <si>
+    <t>C25117</t>
+  </si>
+  <si>
+    <t>470Ω</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>C11702</t>
+  </si>
+  <si>
+    <t>1kΩ</t>
+  </si>
+  <si>
+    <t>R11, R12</t>
+  </si>
+  <si>
+    <t>R16, …, R55</t>
+  </si>
+  <si>
+    <t>C25079</t>
+  </si>
+  <si>
+    <t>120Ω</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>U4, U6</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>U9,…,U13</t>
   </si>
 </sst>
 </file>
@@ -319,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -333,6 +437,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -647,14 +752,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E83B5D-4541-480F-8D66-7615F800B320}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="20.88671875" customWidth="1"/>
     <col min="3" max="3" width="14.88671875" customWidth="1"/>
     <col min="4" max="4" width="15.88671875" customWidth="1"/>
     <col min="5" max="5" width="43" customWidth="1"/>
@@ -691,6 +797,9 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="29.4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
       <c r="B4" t="s">
         <v>21</v>
       </c>
@@ -711,23 +820,26 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>109</v>
+      </c>
       <c r="B5" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.35">
@@ -753,7 +865,7 @@
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
@@ -776,7 +888,7 @@
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>108</v>
       </c>
       <c r="B8" t="s">
         <v>22</v>
@@ -794,15 +906,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>42</v>
+    <row r="9" spans="1:7" ht="29.4" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>94</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>29</v>
@@ -811,7 +923,7 @@
         <v>30</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>28</v>
@@ -819,157 +931,338 @@
     </row>
     <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>95</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" t="s">
-        <v>33</v>
+        <v>76</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>36</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F10" s="2"/>
       <c r="G10" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="43.8" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
-        <v>68</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>98</v>
       </c>
       <c r="B11" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>39</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
       <c r="G11" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>46</v>
+        <v>99</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>102</v>
       </c>
       <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="58.2" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="29.4" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
       <c r="C15" s="2" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
         <v>21</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" t="s">
+        <v>66</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" t="s">
         <v>70</v>
       </c>
-      <c r="D16" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="2" t="s">
+      <c r="G26" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>